<commit_message>
Update reports for demo
</commit_message>
<xml_diff>
--- a/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/lighting_test_demo.xlsx
+++ b/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/lighting_test_demo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ruleset-checking-tool\rct229\ruletest_engine\ruletest_jsons\ruletest_spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcne591\Documents\Github\ruleset-checking-tool\rct229\ruletest_engine\ruletest_jsons\ruletest_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865FB7E8-6594-4B55-9CFE-D1D76E4B3B95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFCE517-6DB8-4EA0-8DC6-CC81D8BE4C7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
   </bookViews>
   <sheets>
     <sheet name="TCDs" sheetId="4" r:id="rId1"/>

</xml_diff>